<commit_message>
Updated BOM (re-runned KiCost to check today's price)
</commit_message>
<xml_diff>
--- a/kicad/hack-Digi-BOM.xlsx
+++ b/kicad/hack-Digi-BOM.xlsx
@@ -383,7 +383,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="159">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -796,6 +796,9 @@
     <t>998-MIC5528-3.3YMTTR</t>
   </si>
   <si>
+    <t>81-LQM18PN4R7MFRL</t>
+  </si>
+  <si>
     <t>603-CC603KRX7R9BB104</t>
   </si>
   <si>
@@ -841,7 +844,7 @@
     <t>67T2259</t>
   </si>
   <si>
-    <t>90R7669</t>
+    <t>06R5243</t>
   </si>
   <si>
     <t>68R4788</t>
@@ -1002,7 +1005,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="102">
+  <dxfs count="106">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF80FF80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF80FF80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF80FF80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF80FF80"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2017,10 +2048,10 @@
   <dimension ref="A1:AA55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="6" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="M32" sqref="M32"/>
+      <selection pane="bottomRight" activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2076,7 @@
         <v>96</v>
       </c>
       <c r="I1" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
@@ -2054,19 +2085,19 @@
       </c>
       <c r="I2" s="3">
         <f ca="1">SUM(I7:I30)</f>
-        <v>152.54400000000001</v>
+        <v>171.97319999999999</v>
       </c>
       <c r="M2" s="3">
         <f>SUM(M7:M30)</f>
-        <v>173.17600000000004</v>
+        <v>182.12880000000004</v>
       </c>
       <c r="S2" s="3">
         <f>SUM(S7:S30)</f>
-        <v>175.38000000000002</v>
+        <v>195.82499999999999</v>
       </c>
       <c r="Y2" s="3">
         <f>SUM(Y7:Y30)</f>
-        <v>131.04</v>
+        <v>137.80199999999999</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
@@ -2075,7 +2106,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TotalCost/BoardQty</f>
-        <v>7.6272000000000002</v>
+        <v>8.1891999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="18.75" x14ac:dyDescent="0.25">
@@ -2107,7 +2138,7 @@
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
       <c r="V5" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="W5" s="11"/>
       <c r="X5" s="11"/>
@@ -2213,7 +2244,7 @@
       </c>
       <c r="G7">
         <f>BoardQty*2</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" ref="H7:H30" ca="1" si="0">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -2221,10 +2252,10 @@
       </c>
       <c r="I7" s="6">
         <f t="shared" ref="I7:I30" ca="1" si="1">IFERROR(G7*H7,"")</f>
-        <v>5.36</v>
+        <v>5.6280000000000001</v>
       </c>
       <c r="J7">
-        <v>147875</v>
+        <v>146304</v>
       </c>
       <c r="L7" s="6">
         <f>IFERROR(LOOKUP(IF(K7="",G7,K7),{0,1,10,25,50,100,250,500,1000,2000,4000,10000,14000,50000,100000},{0,0.28,0.237,0.1628,0.1332,0.1184,0.0888,0.07844,0.06956,0.0592,0.05476,0.0518,0.04914,0.0444,0.03922}),"")</f>
@@ -2232,7 +2263,7 @@
       </c>
       <c r="M7" s="6">
         <f>IFERROR(IF(K7="",G7,K7)*L7,"")</f>
-        <v>6.5120000000000005</v>
+        <v>6.8376000000000001</v>
       </c>
       <c r="N7" t="s">
         <v>104</v>
@@ -2241,7 +2272,7 @@
         <v>105</v>
       </c>
       <c r="P7">
-        <v>23090</v>
+        <v>22886</v>
       </c>
       <c r="R7" s="6">
         <f>IFERROR(LOOKUP(IF(Q7="",G7,Q7),{0,1,10,100,1000,2000,10000,24000,50000,100000},{0,0.279,0.134,0.078,0.07,0.055,0.05,0.048,0.045,0.04}),"")</f>
@@ -2249,7 +2280,7 @@
       </c>
       <c r="S7" s="6">
         <f>IFERROR(IF(Q7="",G7,Q7)*R7,"")</f>
-        <v>5.36</v>
+        <v>5.6280000000000001</v>
       </c>
       <c r="T7" t="s">
         <v>124</v>
@@ -2258,7 +2289,7 @@
         <v>105</v>
       </c>
       <c r="V7">
-        <v>1079</v>
+        <v>829</v>
       </c>
       <c r="X7" s="6">
         <f>IFERROR(LOOKUP(IF(W7="",G7,W7),{0,1,10,25,50,100,250,500,1000},{0,0.318,0.296,0.195,0.162,0.138,0.111,0.098,0.087}),"")</f>
@@ -2266,10 +2297,10 @@
       </c>
       <c r="Y7" s="6">
         <f>IFERROR(IF(W7="",G7,W7)*X7,"")</f>
-        <v>7.8000000000000007</v>
+        <v>8.19</v>
       </c>
       <c r="Z7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AA7" s="7" t="s">
         <v>105</v>
@@ -2290,7 +2321,7 @@
       </c>
       <c r="G8">
         <f t="shared" ref="G8:G15" si="2">BoardQty*1</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -2298,10 +2329,10 @@
       </c>
       <c r="I8" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7199999999999998</v>
+        <v>3.9060000000000001</v>
       </c>
       <c r="J8">
-        <v>324049</v>
+        <v>294147</v>
       </c>
       <c r="L8" s="6">
         <f>IFERROR(LOOKUP(IF(K8="",G8,K8),{0,1,10,100,250,500,1000,3000,6000,15000,30000,75000,150000},{0,0.24,0.186,0.1015,0.06768,0.05752,0.04399,0.03892,0.03384,0.03046,0.02707,0.02453,0.02284}),"")</f>
@@ -2309,7 +2340,7 @@
       </c>
       <c r="M8" s="6">
         <f>IFERROR(IF(K8="",G8,K8)*L8,"")</f>
-        <v>3.7199999999999998</v>
+        <v>3.9060000000000001</v>
       </c>
       <c r="N8" t="s">
         <v>106</v>
@@ -2318,7 +2349,7 @@
         <v>105</v>
       </c>
       <c r="P8">
-        <v>54863</v>
+        <v>47288</v>
       </c>
       <c r="R8" s="6">
         <f>IFERROR(LOOKUP(IF(Q8="",G8,Q8),{0,1,10,100,1000,3000,9000,24000,45000,99000},{0,0.299,0.232,0.073,0.056,0.043,0.038,0.034,0.031,0.028}),"")</f>
@@ -2326,7 +2357,7 @@
       </c>
       <c r="S8" s="6">
         <f>IFERROR(IF(Q8="",G8,Q8)*R8,"")</f>
-        <v>4.6400000000000006</v>
+        <v>4.8719999999999999</v>
       </c>
       <c r="T8" t="s">
         <v>125</v>
@@ -2335,7 +2366,7 @@
         <v>105</v>
       </c>
       <c r="V8">
-        <v>1969</v>
+        <v>1769</v>
       </c>
       <c r="X8" s="6">
         <f>IFERROR(LOOKUP(IF(W8="",G8,W8),{0,1,10,100,500},{0,0.522,0.434,0.347,0.324}),"")</f>
@@ -2343,10 +2374,10 @@
       </c>
       <c r="Y8" s="6">
         <f>IFERROR(IF(W8="",G8,W8)*X8,"")</f>
-        <v>8.68</v>
+        <v>9.1140000000000008</v>
       </c>
       <c r="Z8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AA8" s="7" t="s">
         <v>105</v>
@@ -2367,7 +2398,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -2375,10 +2406,10 @@
       </c>
       <c r="I9" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9.84</v>
+        <v>10.332000000000001</v>
       </c>
       <c r="J9">
-        <v>10888</v>
+        <v>10793</v>
       </c>
       <c r="L9" s="6">
         <f>IFERROR(LOOKUP(IF(K9="",G9,K9),{0,1,10,25,100,250,500,1000,3000,6000,15000,30000,75000,150000},{0,0.67,0.569,0.498,0.4264,0.36984,0.31326,0.2415,0.2139,0.2001,0.1863,0.17664,0.1725,0.1656}),"")</f>
@@ -2386,7 +2417,7 @@
       </c>
       <c r="M9" s="6">
         <f>IFERROR(IF(K9="",G9,K9)*L9,"")</f>
-        <v>11.379999999999999</v>
+        <v>11.948999999999998</v>
       </c>
       <c r="N9" t="s">
         <v>107</v>
@@ -2395,7 +2426,7 @@
         <v>105</v>
       </c>
       <c r="P9">
-        <v>13021</v>
+        <v>12154</v>
       </c>
       <c r="R9" s="6">
         <f>IFERROR(LOOKUP(IF(Q9="",G9,Q9),{0,1,10,100,1000,3000,9000,24000},{0,0.651,0.492,0.308,0.232,0.197,0.183,0.18}),"")</f>
@@ -2403,7 +2434,7 @@
       </c>
       <c r="S9" s="6">
         <f>IFERROR(IF(Q9="",G9,Q9)*R9,"")</f>
-        <v>9.84</v>
+        <v>10.332000000000001</v>
       </c>
       <c r="T9" t="s">
         <v>126</v>
@@ -2412,7 +2443,7 @@
         <v>105</v>
       </c>
       <c r="V9">
-        <v>7937</v>
+        <v>7927</v>
       </c>
       <c r="X9" s="6">
         <f>IFERROR(LOOKUP(IF(W9="",G9,W9),{0,1,25,100,250,500,1000,3000,9000},{0,0.66,0.483,0.304,0.294,0.286,0.235,0.201,0.187}),"")</f>
@@ -2420,10 +2451,10 @@
       </c>
       <c r="Y9" s="6">
         <f>IFERROR(IF(W9="",G9,W9)*X9,"")</f>
-        <v>13.200000000000001</v>
+        <v>13.860000000000001</v>
       </c>
       <c r="Z9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AA9" s="7" t="s">
         <v>105</v>
@@ -2444,7 +2475,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -2452,18 +2483,18 @@
       </c>
       <c r="I10" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38</v>
+        <v>0.39899999999999997</v>
       </c>
       <c r="J10">
-        <v>45701</v>
+        <v>45511</v>
       </c>
       <c r="L10" s="6">
-        <f>IFERROR(LOOKUP(IF(K10="",G10,K10),{0,1,10,25,100,250,500,1000,4000,8000,12000,28000,100000},{0,0.1,0.024,0.0172,0.0112,0.0092,0.00786,0.00612,0.00469,0.00428,0.00408,0.00388,0.00281}),"")</f>
-        <v>2.4E-2</v>
+        <f>IFERROR(LOOKUP(IF(K10="",G10,K10),{0,1,10,25,100,250,500,1000,4000,8000,12000,28000,100000},{0,0.1,0.026,0.0184,0.0118,0.00964,0.00824,0.00643,0.00493,0.0045,0.00428,0.00407,0.00295}),"")</f>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="M10" s="6">
         <f>IFERROR(IF(K10="",G10,K10)*L10,"")</f>
-        <v>0.48</v>
+        <v>0.54599999999999993</v>
       </c>
       <c r="N10" t="s">
         <v>108</v>
@@ -2472,7 +2503,7 @@
         <v>105</v>
       </c>
       <c r="P10">
-        <v>48853</v>
+        <v>48553</v>
       </c>
       <c r="R10" s="6">
         <f>IFERROR(LOOKUP(IF(Q10="",G10,Q10),{0,1,10,100,1000,4000,8000,100000},{0,0.099,0.019,0.009,0.007,0.005,0.004,0.003}),"")</f>
@@ -2480,7 +2511,7 @@
       </c>
       <c r="S10" s="6">
         <f>IFERROR(IF(Q10="",G10,Q10)*R10,"")</f>
-        <v>0.38</v>
+        <v>0.39899999999999997</v>
       </c>
       <c r="T10" t="s">
         <v>127</v>
@@ -2489,7 +2520,7 @@
         <v>105</v>
       </c>
       <c r="V10">
-        <v>4690</v>
+        <v>2940</v>
       </c>
       <c r="X10" s="6">
         <f>IFERROR(LOOKUP(IF(W10="",G10,W10),{0,1,10,25,100,250,500,1000},{0,0.103,0.046,0.033,0.021,0.017,0.015,0.012}),"")</f>
@@ -2497,10 +2528,10 @@
       </c>
       <c r="Y10" s="6">
         <f>IFERROR(IF(W10="",G10,W10)*X10,"")</f>
-        <v>0.91999999999999993</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="Z10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AA10" s="7" t="s">
         <v>105</v>
@@ -2521,7 +2552,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -2529,10 +2560,10 @@
       </c>
       <c r="I11" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>4.24</v>
+        <v>4.452</v>
       </c>
       <c r="J11">
-        <v>4526</v>
+        <v>526</v>
       </c>
       <c r="L11" s="6">
         <f>IFERROR(LOOKUP(IF(K11="",G11,K11),{0,1,10,50,100,500,2000,4000,6000,10000,20000},{0,0.54,0.51,0.4786,0.4466,0.3509,0.1914,0.18502,0.17864,0.17226,0.16397}),"")</f>
@@ -2540,7 +2571,7 @@
       </c>
       <c r="M11" s="6">
         <f>IFERROR(IF(K11="",G11,K11)*L11,"")</f>
-        <v>10.199999999999999</v>
+        <v>10.71</v>
       </c>
       <c r="N11" t="s">
         <v>109</v>
@@ -2557,7 +2588,7 @@
       </c>
       <c r="S11" s="6">
         <f>IFERROR(IF(Q11="",G11,Q11)*R11,"")</f>
-        <v>9.44</v>
+        <v>9.911999999999999</v>
       </c>
       <c r="T11" t="s">
         <v>128</v>
@@ -2574,10 +2605,10 @@
       </c>
       <c r="Y11" s="6">
         <f>IFERROR(IF(W11="",G11,W11)*X11,"")</f>
-        <v>4.24</v>
+        <v>4.452</v>
       </c>
       <c r="Z11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AA11" s="7" t="s">
         <v>105</v>
@@ -2595,7 +2626,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -2621,7 +2652,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H13" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -2629,10 +2660,10 @@
       </c>
       <c r="I13" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>60.8</v>
+        <v>63.84</v>
       </c>
       <c r="J13">
-        <v>911</v>
+        <v>907</v>
       </c>
       <c r="L13" s="6">
         <f>IFERROR(LOOKUP(IF(K13="",G13,K13),{0,1,10,100,250,500,1000},{0,5.03,4.493,3.6845,3.325,2.98352,2.51622}),"")</f>
@@ -2640,7 +2671,7 @@
       </c>
       <c r="M13" s="6">
         <f>IFERROR(IF(K13="",G13,K13)*L13,"")</f>
-        <v>89.860000000000014</v>
+        <v>94.353000000000009</v>
       </c>
       <c r="N13" t="s">
         <v>110</v>
@@ -2657,7 +2688,7 @@
       </c>
       <c r="S13" s="6">
         <f>IFERROR(IF(Q13="",G13,Q13)*R13,"")</f>
-        <v>88.6</v>
+        <v>93.03</v>
       </c>
       <c r="T13" t="s">
         <v>129</v>
@@ -2674,10 +2705,10 @@
       </c>
       <c r="Y13" s="6">
         <f>IFERROR(IF(W13="",G13,W13)*X13,"")</f>
-        <v>60.8</v>
+        <v>63.84</v>
       </c>
       <c r="Z13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AA13" s="7" t="s">
         <v>105</v>
@@ -2698,18 +2729,18 @@
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H14" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10299999999999999</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="I14" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>2.06</v>
+        <v>2.121</v>
       </c>
       <c r="J14">
-        <v>315669</v>
+        <v>309192</v>
       </c>
       <c r="L14" s="6">
         <f>IFERROR(LOOKUP(IF(K14="",G14,K14),{0,1,10,50,100,250,500,1000,4000,8000,12000},{0,0.23,0.175,0.1252,0.1126,0.09508,0.08508,0.07257,0.0637,0.05847,0.05688}),"")</f>
@@ -2717,7 +2748,7 @@
       </c>
       <c r="M14" s="6">
         <f>IFERROR(IF(K14="",G14,K14)*L14,"")</f>
-        <v>3.5</v>
+        <v>3.6749999999999998</v>
       </c>
       <c r="N14" t="s">
         <v>111</v>
@@ -2726,7 +2757,7 @@
         <v>105</v>
       </c>
       <c r="P14">
-        <v>82453</v>
+        <v>80667</v>
       </c>
       <c r="R14" s="6">
         <f>IFERROR(LOOKUP(IF(Q14="",G14,Q14),{0,1,10,100,500,1000,4000,8000},{0,0.227,0.124,0.095,0.085,0.072,0.063,0.06}),"")</f>
@@ -2734,7 +2765,7 @@
       </c>
       <c r="S14" s="6">
         <f>IFERROR(IF(Q14="",G14,Q14)*R14,"")</f>
-        <v>2.48</v>
+        <v>2.6040000000000001</v>
       </c>
       <c r="T14" t="s">
         <v>130</v>
@@ -2743,18 +2774,18 @@
         <v>105</v>
       </c>
       <c r="V14">
-        <v>6460</v>
+        <v>13079</v>
       </c>
       <c r="X14" s="6">
-        <f>IFERROR(LOOKUP(IF(W14="",G14,W14),{0,1,50,100,500,1000,2500,5000,10000},{0,0.103,0.093,0.075,0.067,0.061,0.056,0.053,0.05}),"")</f>
-        <v>0.10299999999999999</v>
+        <f>IFERROR(LOOKUP(IF(W14="",G14,W14),{0,1,50,100,500,1000,2500,5000,10000},{0,0.101,0.091,0.073,0.065,0.059,0.055,0.052,0.049}),"")</f>
+        <v>0.10100000000000001</v>
       </c>
       <c r="Y14" s="6">
         <f>IFERROR(IF(W14="",G14,W14)*X14,"")</f>
-        <v>2.06</v>
+        <v>2.121</v>
       </c>
       <c r="Z14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA14" s="7" t="s">
         <v>105</v>
@@ -2775,7 +2806,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -2783,10 +2814,10 @@
       </c>
       <c r="I15" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="J15">
-        <v>10581313</v>
+        <v>10065467</v>
       </c>
       <c r="L15" s="6">
         <f>IFERROR(LOOKUP(IF(K15="",G15,K15),{0,1,10,25,100,250,500,1000,2500,5000,10000,25000,50000,125000},{0,0.1,0.014,0.01,0.0057,0.00436,0.00348,0.00257,0.00223,0.00167,0.00145,0.00128,0.00117,0.00115}),"")</f>
@@ -2794,7 +2825,7 @@
       </c>
       <c r="M15" s="6">
         <f>IFERROR(IF(K15="",G15,K15)*L15,"")</f>
-        <v>0.28000000000000003</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="N15" t="s">
         <v>112</v>
@@ -2803,7 +2834,7 @@
         <v>105</v>
       </c>
       <c r="P15">
-        <v>1902372</v>
+        <v>2016779</v>
       </c>
       <c r="R15" s="6">
         <f>IFERROR(LOOKUP(IF(Q15="",G15,Q15),{0,1,10,100,1000,5000,10000},{0,0.099,0.01,0.003,0.002,0.002,0.001}),"")</f>
@@ -2811,7 +2842,7 @@
       </c>
       <c r="S15" s="6">
         <f>IFERROR(IF(Q15="",G15,Q15)*R15,"")</f>
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="T15" t="s">
         <v>131</v>
@@ -2820,7 +2851,7 @@
         <v>105</v>
       </c>
       <c r="V15">
-        <v>64</v>
+        <v>4809</v>
       </c>
       <c r="X15" s="6">
         <f>IFERROR(LOOKUP(IF(W15="",G15,W15),{0,1,10,25,100,250,1000},{0,0.09,0.015,0.011,0.006,0.004,0.003}),"")</f>
@@ -2828,10 +2859,10 @@
       </c>
       <c r="Y15" s="6">
         <f>IFERROR(IF(W15="",G15,W15)*X15,"")</f>
-        <v>0.3</v>
+        <v>0.315</v>
       </c>
       <c r="Z15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AA15" s="7" t="s">
         <v>105</v>
@@ -2849,7 +2880,7 @@
       </c>
       <c r="G16">
         <f>BoardQty*3</f>
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H16" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -2875,7 +2906,7 @@
       </c>
       <c r="G17">
         <f>BoardQty*1</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H17" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -2883,10 +2914,10 @@
       </c>
       <c r="I17" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>5.36</v>
+        <v>5.6280000000000001</v>
       </c>
       <c r="J17">
-        <v>41300</v>
+        <v>39749</v>
       </c>
       <c r="L17" s="6">
         <f>IFERROR(LOOKUP(IF(K17="",G17,K17),{0,1,10,25,50,100,250,500,1000,2900,5800},{0,0.28,0.268,0.2588,0.2494,0.2356,0.22176,0.21252,0.1617,0.147,0.1218}),"")</f>
@@ -2894,7 +2925,7 @@
       </c>
       <c r="M17" s="6">
         <f>IFERROR(IF(K17="",G17,K17)*L17,"")</f>
-        <v>5.36</v>
+        <v>5.6280000000000001</v>
       </c>
       <c r="N17" t="s">
         <v>113</v>
@@ -2903,7 +2934,7 @@
         <v>105</v>
       </c>
       <c r="P17">
-        <v>6271</v>
+        <v>5616</v>
       </c>
       <c r="R17" s="6">
         <f>IFERROR(LOOKUP(IF(Q17="",G17,Q17),{0,1,25,50,100,250,500,1000,2900,5800},{0,0.279,0.257,0.249,0.234,0.22,0.211,0.191,0.171,0.128}),"")</f>
@@ -2911,7 +2942,7 @@
       </c>
       <c r="S17" s="6">
         <f>IFERROR(IF(Q17="",G17,Q17)*R17,"")</f>
-        <v>5.58</v>
+        <v>5.8590000000000009</v>
       </c>
       <c r="T17" t="s">
         <v>132</v>
@@ -2935,7 +2966,7 @@
       </c>
       <c r="G18">
         <f>BoardQty*1</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H18" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -2943,10 +2974,10 @@
       </c>
       <c r="I18" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>6.22</v>
+        <v>6.5309999999999997</v>
       </c>
       <c r="J18">
-        <v>150329</v>
+        <v>147639</v>
       </c>
       <c r="L18" s="6">
         <f>IFERROR(LOOKUP(IF(K18="",G18,K18),{0,1,10,25,50,100,250,500,1200,2400,6000,8400,12000,30000,60000},{0,0.46,0.433,0.3712,0.3156,0.3032,0.27224,0.25988,0.19688,0.18,0.16875,0.1575,0.15188,0.14963,0.14625}),"")</f>
@@ -2954,7 +2985,7 @@
       </c>
       <c r="M18" s="6">
         <f>IFERROR(IF(K18="",G18,K18)*L18,"")</f>
-        <v>8.66</v>
+        <v>9.093</v>
       </c>
       <c r="N18" t="s">
         <v>114</v>
@@ -2963,15 +2994,15 @@
         <v>105</v>
       </c>
       <c r="P18">
-        <v>21362</v>
+        <v>20536</v>
       </c>
       <c r="R18" s="6">
-        <f>IFERROR(LOOKUP(IF(Q18="",G18,Q18),{0,1,10,100,500,1200,2400,4800,9600},{0,0.468,0.322,0.277,0.264,0.201,0.183,0.162,0.158}),"")</f>
+        <f>IFERROR(LOOKUP(IF(Q18="",G18,Q18),{0,1,10,100,500,1200,2400,4800},{0,0.468,0.322,0.277,0.264,0.201,0.183,0.174}),"")</f>
         <v>0.32200000000000001</v>
       </c>
       <c r="S18" s="6">
         <f>IFERROR(IF(Q18="",G18,Q18)*R18,"")</f>
-        <v>6.44</v>
+        <v>6.7620000000000005</v>
       </c>
       <c r="T18" t="s">
         <v>133</v>
@@ -2980,7 +3011,7 @@
         <v>105</v>
       </c>
       <c r="V18">
-        <v>9471</v>
+        <v>8721</v>
       </c>
       <c r="X18" s="6">
         <f>IFERROR(LOOKUP(IF(W18="",G18,W18),{0,1,10,25,50,100,250,500,1000},{0,0.345,0.311,0.276,0.265,0.242,0.23,0.191,0.173}),"")</f>
@@ -2988,10 +3019,10 @@
       </c>
       <c r="Y18" s="6">
         <f>IFERROR(IF(W18="",G18,W18)*X18,"")</f>
-        <v>6.22</v>
+        <v>6.5309999999999997</v>
       </c>
       <c r="Z18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AA18" s="7" t="s">
         <v>105</v>
@@ -3012,7 +3043,7 @@
       </c>
       <c r="G19">
         <f>BoardQty*1</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H19" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -3020,7 +3051,7 @@
       </c>
       <c r="I19" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>23.1</v>
       </c>
       <c r="P19">
         <v>149</v>
@@ -3031,7 +3062,7 @@
       </c>
       <c r="S19" s="6">
         <f>IFERROR(IF(Q19="",G19,Q19)*R19,"")</f>
-        <v>22</v>
+        <v>23.1</v>
       </c>
       <c r="T19" t="s">
         <v>134</v>
@@ -3052,7 +3083,7 @@
       </c>
       <c r="G20">
         <f>BoardQty*1</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H20" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -3078,26 +3109,26 @@
       </c>
       <c r="G21">
         <f>BoardQty*2</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H21" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0799999999999998E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="I21" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>2.032</v>
+        <v>2.1839999999999997</v>
       </c>
       <c r="J21">
-        <v>6084</v>
+        <v>5474</v>
       </c>
       <c r="L21" s="6">
-        <f>IFERROR(LOOKUP(IF(K21="",G21,K21),{0,1,10,25,100,250,500,1000,4000,8000,12000,28000,100000},{0,0.1,0.072,0.0508,0.0329,0.02692,0.02302,0.01794,0.01376,0.01256,0.01196,0.01136,0.00822}),"")</f>
-        <v>5.0799999999999998E-2</v>
+        <f>IFERROR(LOOKUP(IF(K21="",G21,K21),{0,1,10,25,100,250,500,1000,4000,8000,12000,28000,100000},{0,0.1,0.075,0.0532,0.0345,0.02824,0.02418,0.01884,0.01444,0.01319,0.01256,0.01193,0.00863}),"")</f>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="M21" s="6">
         <f>IFERROR(IF(K21="",G21,K21)*L21,"")</f>
-        <v>2.032</v>
+        <v>2.2343999999999999</v>
       </c>
       <c r="N21" t="s">
         <v>115</v>
@@ -3106,15 +3137,15 @@
         <v>105</v>
       </c>
       <c r="P21">
-        <v>4215</v>
+        <v>3965</v>
       </c>
       <c r="R21" s="6">
         <f>IFERROR(LOOKUP(IF(Q21="",G21,Q21),{0,1,10,100,1000,4000,24000,48000,100000},{0,0.099,0.052,0.024,0.019,0.013,0.012,0.011,0.009}),"")</f>
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="S21" s="6">
-        <f>IFERROR(IF(Q21="",G21,Q21)*R21,"")</f>
-        <v>2.08</v>
+        <f t="shared" ref="S21:S26" si="3">IFERROR(IF(Q21="",G21,Q21)*R21,"")</f>
+        <v>2.1839999999999997</v>
       </c>
       <c r="T21" t="s">
         <v>135</v>
@@ -3123,18 +3154,18 @@
         <v>105</v>
       </c>
       <c r="V21">
-        <v>3335</v>
+        <v>3272</v>
       </c>
       <c r="X21" s="6">
-        <f>IFERROR(LOOKUP(IF(W21="",G21,W21),{0,1,10,100,250,500,1000},{0,0.16,0.11,0.053,0.044,0.037,0.03}),"")</f>
-        <v>0.11</v>
+        <f>IFERROR(LOOKUP(IF(W21="",G21,W21),{0,1,10,50,100,250,500,1000},{0,0.164,0.116,0.062,0.049,0.042,0.036,0.03}),"")</f>
+        <v>0.11600000000000001</v>
       </c>
       <c r="Y21" s="6">
         <f>IFERROR(IF(W21="",G21,W21)*X21,"")</f>
-        <v>4.4000000000000004</v>
+        <v>4.8719999999999999</v>
       </c>
       <c r="Z21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AA21" s="7" t="s">
         <v>105</v>
@@ -3155,7 +3186,7 @@
       </c>
       <c r="G22">
         <f>BoardQty*1</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H22" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -3163,10 +3194,10 @@
       </c>
       <c r="I22" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>3.74</v>
+        <v>3.927</v>
       </c>
       <c r="J22">
-        <v>5000</v>
+        <v>4970</v>
       </c>
       <c r="L22" s="6">
         <f>IFERROR(LOOKUP(IF(K22="",G22,K22),{0,1,25,100,4500,5000},{0,0.19,0.16,0.14,0.24,0.14}),"")</f>
@@ -3174,7 +3205,7 @@
       </c>
       <c r="M22" s="6">
         <f>IFERROR(IF(K22="",G22,K22)*L22,"")</f>
-        <v>3.8</v>
+        <v>3.99</v>
       </c>
       <c r="N22" t="s">
         <v>116</v>
@@ -3183,15 +3214,15 @@
         <v>105</v>
       </c>
       <c r="P22">
-        <v>4797</v>
+        <v>4794</v>
       </c>
       <c r="R22" s="6">
         <f>IFERROR(LOOKUP(IF(Q22="",G22,Q22),{0,1,10,25,100,5000},{0,0.197,0.187,0.158,0.138,0.138}),"")</f>
         <v>0.187</v>
       </c>
       <c r="S22" s="6">
-        <f>IFERROR(IF(Q22="",G22,Q22)*R22,"")</f>
-        <v>3.74</v>
+        <f t="shared" si="3"/>
+        <v>3.927</v>
       </c>
       <c r="T22" t="s">
         <v>136</v>
@@ -3215,15 +3246,32 @@
       </c>
       <c r="G23">
         <f>BoardQty*1</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H23" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="I23" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>5.838000000000001</v>
+      </c>
+      <c r="P23">
+        <v>2507</v>
+      </c>
+      <c r="R23" s="6">
+        <f>IFERROR(LOOKUP(IF(Q23="",G23,Q23),{0,1,10,100,1000,4000,8000,24000,48000,100000},{0,0.395,0.278,0.207,0.182,0.135,0.123,0.12,0.116,0.111}),"")</f>
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="S23" s="6">
+        <f t="shared" si="3"/>
+        <v>5.838000000000001</v>
+      </c>
+      <c r="T23" t="s">
+        <v>137</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
@@ -3241,26 +3289,26 @@
       </c>
       <c r="G24">
         <f>BoardQty*4</f>
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H24" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9199999999999998E-2</v>
+        <v>0.02</v>
       </c>
       <c r="I24" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5359999999999998</v>
+        <v>1.68</v>
       </c>
       <c r="J24">
-        <v>1823681</v>
+        <v>1594945</v>
       </c>
       <c r="L24" s="6">
-        <f>IFERROR(LOOKUP(IF(K24="",G24,K24),{0,1,10,25,100,250,500,1000,4000,8000,12000,28000,100000},{0,0.1,0.027,0.0192,0.0125,0.0102,0.00874,0.00681,0.00522,0.00477,0.00454,0.00431,0.00312}),"")</f>
-        <v>1.9199999999999998E-2</v>
+        <f>IFERROR(LOOKUP(IF(K24="",G24,K24),{0,1,10,25,100,250,500,1000,4000,8000,12000,28000,100000},{0,0.1,0.029,0.0204,0.0131,0.01072,0.00918,0.00715,0.00548,0.00501,0.00477,0.00453,0.00328}),"")</f>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="M24" s="6">
         <f>IFERROR(IF(K24="",G24,K24)*L24,"")</f>
-        <v>1.5359999999999998</v>
+        <v>1.7136</v>
       </c>
       <c r="N24" t="s">
         <v>117</v>
@@ -3269,24 +3317,24 @@
         <v>105</v>
       </c>
       <c r="P24">
-        <v>696803</v>
+        <v>589899</v>
       </c>
       <c r="R24" s="6">
         <f>IFERROR(LOOKUP(IF(Q24="",G24,Q24),{0,1,10,100,1000,4000,48000},{0,0.099,0.02,0.009,0.007,0.005,0.004}),"")</f>
         <v>0.02</v>
       </c>
       <c r="S24" s="6">
-        <f>IFERROR(IF(Q24="",G24,Q24)*R24,"")</f>
-        <v>1.6</v>
+        <f t="shared" si="3"/>
+        <v>1.68</v>
       </c>
       <c r="T24" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="U24" s="7" t="s">
         <v>105</v>
       </c>
       <c r="V24">
-        <v>4188</v>
+        <v>2488</v>
       </c>
       <c r="X24" s="6">
         <f>IFERROR(LOOKUP(IF(W24="",G24,W24),{0,1,10,25,100,250,500,1000},{0,0.1,0.036,0.026,0.014,0.011,0.008,0.006}),"")</f>
@@ -3294,10 +3342,10 @@
       </c>
       <c r="Y24" s="6">
         <f>IFERROR(IF(W24="",G24,W24)*X24,"")</f>
-        <v>2.08</v>
+        <v>2.1839999999999997</v>
       </c>
       <c r="Z24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AA24" s="7" t="s">
         <v>105</v>
@@ -3318,7 +3366,7 @@
       </c>
       <c r="G25">
         <f>BoardQty*1</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H25" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -3326,10 +3374,10 @@
       </c>
       <c r="I25" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="J25">
-        <v>1441547</v>
+        <v>1335355</v>
       </c>
       <c r="L25" s="6">
         <f>IFERROR(LOOKUP(IF(K25="",G25,K25),{0,1,10,25,100,250,500,1000,2500,5000,10000,25000,50000,125000},{0,0.1,0.014,0.01,0.0057,0.00436,0.00348,0.00257,0.00223,0.00167,0.00145,0.00128,0.00117,0.00115}),"")</f>
@@ -3337,7 +3385,7 @@
       </c>
       <c r="M25" s="6">
         <f>IFERROR(IF(K25="",G25,K25)*L25,"")</f>
-        <v>0.28000000000000003</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="N25" t="s">
         <v>118</v>
@@ -3346,24 +3394,24 @@
         <v>105</v>
       </c>
       <c r="P25">
-        <v>220770</v>
+        <v>150640</v>
       </c>
       <c r="R25" s="6">
         <f>IFERROR(LOOKUP(IF(Q25="",G25,Q25),{0,1,10,100,1000,5000,10000},{0,0.099,0.01,0.003,0.002,0.002,0.001}),"")</f>
         <v>0.01</v>
       </c>
       <c r="S25" s="6">
-        <f>IFERROR(IF(Q25="",G25,Q25)*R25,"")</f>
-        <v>0.2</v>
+        <f t="shared" si="3"/>
+        <v>0.21</v>
       </c>
       <c r="T25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="U25" s="7" t="s">
         <v>105</v>
       </c>
       <c r="V25">
-        <v>3513</v>
+        <v>4058</v>
       </c>
       <c r="X25" s="6">
         <f>IFERROR(LOOKUP(IF(W25="",G25,W25),{0,1,10,25,100,250,1000},{0,0.09,0.015,0.011,0.006,0.004,0.003}),"")</f>
@@ -3371,16 +3419,16 @@
       </c>
       <c r="Y25" s="6">
         <f>IFERROR(IF(W25="",G25,W25)*X25,"")</f>
-        <v>0.3</v>
+        <v>0.315</v>
       </c>
       <c r="Z25" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AA25" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -3395,15 +3443,32 @@
       </c>
       <c r="G26">
         <f>BoardQty*1</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H26" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="I26" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>5.838000000000001</v>
+      </c>
+      <c r="P26">
+        <v>2507</v>
+      </c>
+      <c r="R26" s="6">
+        <f>IFERROR(LOOKUP(IF(Q26="",G26,Q26),{0,1,10,100,1000,4000,8000,24000,48000,100000},{0,0.395,0.278,0.207,0.182,0.135,0.123,0.12,0.116,0.111}),"")</f>
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="S26" s="6">
+        <f t="shared" si="3"/>
+        <v>5.838000000000001</v>
+      </c>
+      <c r="T26" t="s">
+        <v>137</v>
+      </c>
+      <c r="U26" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
@@ -3421,7 +3486,7 @@
       </c>
       <c r="G27">
         <f>BoardQty*2</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H27" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -3429,7 +3494,7 @@
       </c>
       <c r="I27" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>12.44</v>
+        <v>13.061999999999999</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -3440,7 +3505,7 @@
       </c>
       <c r="M27" s="6">
         <f>IFERROR(IF(K27="",G27,K27)*L27,"")</f>
-        <v>12.44</v>
+        <v>13.061999999999999</v>
       </c>
       <c r="N27" t="s">
         <v>119</v>
@@ -3464,7 +3529,7 @@
       </c>
       <c r="G28">
         <f>BoardQty*2</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H28" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -3472,10 +3537,10 @@
       </c>
       <c r="I28" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.08</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="J28">
-        <v>634473</v>
+        <v>547143</v>
       </c>
       <c r="L28" s="6">
         <f>IFERROR(LOOKUP(IF(K28="",G28,K28),{0,1,10,25,100,250,500,1000,2500,5000,10000,25000,50000,125000},{0,0.1,0.014,0.01,0.0057,0.00436,0.00348,0.00257,0.00223,0.00167,0.00145,0.00128,0.00117,0.00115}),"")</f>
@@ -3483,7 +3548,7 @@
       </c>
       <c r="M28" s="6">
         <f>IFERROR(IF(K28="",G28,K28)*L28,"")</f>
-        <v>0.4</v>
+        <v>0.42</v>
       </c>
       <c r="N28" t="s">
         <v>120</v>
@@ -3492,7 +3557,7 @@
         <v>105</v>
       </c>
       <c r="P28">
-        <v>2084</v>
+        <v>132614</v>
       </c>
       <c r="R28" s="6">
         <f>IFERROR(LOOKUP(IF(Q28="",G28,Q28),{0,1,10,100,1000,5000,10000},{0,0.099,0.01,0.003,0.002,0.002,0.001}),"")</f>
@@ -3500,16 +3565,16 @@
       </c>
       <c r="S28" s="6">
         <f>IFERROR(IF(Q28="",G28,Q28)*R28,"")</f>
-        <v>0.4</v>
+        <v>0.42</v>
       </c>
       <c r="T28" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="U28" s="7" t="s">
         <v>105</v>
       </c>
       <c r="V28">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="X28" s="6">
         <f>IFERROR(LOOKUP(IF(W28="",G28,W28),{0,1,5000,10000,25000},{0,0.002,0.002,0.001,0.001}),"")</f>
@@ -3517,10 +3582,10 @@
       </c>
       <c r="Y28" s="6">
         <f>IFERROR(IF(W28="",G28,W28)*X28,"")</f>
-        <v>0.08</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="Z28" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AA28" s="7" t="s">
         <v>105</v>
@@ -3541,7 +3606,7 @@
       </c>
       <c r="G29">
         <f>BoardQty*1</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H29" s="6">
         <f t="shared" ca="1" si="0"/>
@@ -3549,10 +3614,10 @@
       </c>
       <c r="I29" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>11.44</v>
+        <v>12.011999999999999</v>
       </c>
       <c r="J29">
-        <v>26765</v>
+        <v>18822</v>
       </c>
       <c r="L29" s="6">
         <f>IFERROR(LOOKUP(IF(K29="",G29,K29),{0,1,10,50,100,500,1000,3000,6000,15000},{0,0.71,0.592,0.531,0.4725,0.45,0.378,0.3375,0.32625,0.315}),"")</f>
@@ -3560,7 +3625,7 @@
       </c>
       <c r="M29" s="6">
         <f>IFERROR(IF(K29="",G29,K29)*L29,"")</f>
-        <v>11.84</v>
+        <v>12.431999999999999</v>
       </c>
       <c r="N29" t="s">
         <v>121</v>
@@ -3569,7 +3634,7 @@
         <v>105</v>
       </c>
       <c r="P29">
-        <v>25232</v>
+        <v>25120</v>
       </c>
       <c r="R29" s="6">
         <f>IFERROR(LOOKUP(IF(Q29="",G29,Q29),{0,1,10,50,100,500,1500,3000,6000,9000},{0,0.643,0.572,0.535,0.473,0.374,0.359,0.343,0.331,0.325}),"")</f>
@@ -3577,16 +3642,16 @@
       </c>
       <c r="S29" s="6">
         <f>IFERROR(IF(Q29="",G29,Q29)*R29,"")</f>
-        <v>11.44</v>
+        <v>12.011999999999999</v>
       </c>
       <c r="T29" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="U29" s="7" t="s">
         <v>105</v>
       </c>
       <c r="V29">
-        <v>7896</v>
+        <v>7891</v>
       </c>
       <c r="X29" s="6">
         <f>IFERROR(LOOKUP(IF(W29="",G29,W29),{0,1,10,50,100,500,750,1000},{0,1.05,0.92,0.859,0.76,0.719,0.681,0.601}),"")</f>
@@ -3594,10 +3659,10 @@
       </c>
       <c r="Y29" s="6">
         <f>IFERROR(IF(W29="",G29,W29)*X29,"")</f>
-        <v>18.400000000000002</v>
+        <v>19.32</v>
       </c>
       <c r="Z29" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AA29" s="7" t="s">
         <v>105</v>
@@ -3618,26 +3683,26 @@
       </c>
       <c r="G30">
         <f>BoardQty*2</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H30" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.24E-2</v>
+        <v>2.3599999999999999E-2</v>
       </c>
       <c r="I30" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89600000000000002</v>
+        <v>0.99119999999999997</v>
       </c>
       <c r="J30">
-        <v>38067</v>
+        <v>33300</v>
       </c>
       <c r="L30" s="6">
-        <f>IFERROR(LOOKUP(IF(K30="",G30,K30),{0,1,10,25,100,250,500,1000,4000,8000,12000,28000,100000},{0,0.1,0.032,0.0224,0.0145,0.01188,0.01016,0.00792,0.00607,0.00554,0.00528,0.00502,0.00363}),"")</f>
-        <v>2.24E-2</v>
+        <f>IFERROR(LOOKUP(IF(K30="",G30,K30),{0,1,10,25,100,250,500,1000,4000,8000,12000,28000,100000},{0,0.1,0.033,0.0236,0.0152,0.01248,0.01068,0.00832,0.00638,0.00582,0.00554,0.00527,0.00381}),"")</f>
+        <v>2.3599999999999999E-2</v>
       </c>
       <c r="M30" s="6">
         <f>IFERROR(IF(K30="",G30,K30)*L30,"")</f>
-        <v>0.89600000000000002</v>
+        <v>0.99119999999999997</v>
       </c>
       <c r="N30" t="s">
         <v>122</v>
@@ -3646,7 +3711,7 @@
         <v>105</v>
       </c>
       <c r="P30">
-        <v>23130</v>
+        <v>22668</v>
       </c>
       <c r="R30" s="6">
         <f>IFERROR(LOOKUP(IF(Q30="",G30,Q30),{0,1,10,100,1000,4000,100000},{0,0.099,0.024,0.011,0.008,0.005,0.004}),"")</f>
@@ -3654,16 +3719,16 @@
       </c>
       <c r="S30" s="6">
         <f>IFERROR(IF(Q30="",G30,Q30)*R30,"")</f>
-        <v>0.96</v>
+        <v>1.008</v>
       </c>
       <c r="T30" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="U30" s="7" t="s">
         <v>105</v>
       </c>
       <c r="V30">
-        <v>830</v>
+        <v>800</v>
       </c>
       <c r="X30" s="6">
         <f>IFERROR(LOOKUP(IF(W30="",G30,W30),{0,1,10,25,100,250,500,1000},{0,0.078,0.055,0.039,0.025,0.021,0.018,0.014}),"")</f>
@@ -3671,17 +3736,14 @@
       </c>
       <c r="Y30" s="6">
         <f>IFERROR(IF(W30="",G30,W30)*X30,"")</f>
-        <v>1.56</v>
+        <v>1.6379999999999999</v>
       </c>
       <c r="Z30" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AA30" s="7" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="M31" s="6"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="K32" t="str">
@@ -4603,347 +4665,367 @@
     <mergeCell ref="V5:AA5"/>
   </mergeCells>
   <conditionalFormatting sqref="L10">
-    <cfRule type="cellIs" dxfId="101" priority="7" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="105" priority="7" operator="lessThanOrEqual">
       <formula>H10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="cellIs" dxfId="100" priority="9" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="104" priority="9" operator="lessThanOrEqual">
       <formula>H11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="99" priority="11" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="103" priority="11" operator="lessThanOrEqual">
       <formula>H13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="cellIs" dxfId="98" priority="13" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="102" priority="13" operator="lessThanOrEqual">
       <formula>H14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15">
-    <cfRule type="cellIs" dxfId="97" priority="15" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="101" priority="15" operator="lessThanOrEqual">
       <formula>H15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17">
-    <cfRule type="cellIs" dxfId="96" priority="17" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="100" priority="17" operator="lessThanOrEqual">
       <formula>H17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="cellIs" dxfId="95" priority="19" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="99" priority="19" operator="lessThanOrEqual">
       <formula>H18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="cellIs" dxfId="94" priority="21" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="98" priority="21" operator="lessThanOrEqual">
       <formula>H21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="93" priority="23" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="97" priority="23" operator="lessThanOrEqual">
       <formula>H22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24">
-    <cfRule type="cellIs" dxfId="92" priority="25" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="96" priority="25" operator="lessThanOrEqual">
       <formula>H24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25">
-    <cfRule type="cellIs" dxfId="91" priority="27" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="95" priority="27" operator="lessThanOrEqual">
       <formula>H25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27">
-    <cfRule type="cellIs" dxfId="90" priority="29" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="94" priority="29" operator="lessThanOrEqual">
       <formula>H27</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="cellIs" dxfId="89" priority="31" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="93" priority="31" operator="lessThanOrEqual">
       <formula>H28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L29">
-    <cfRule type="cellIs" dxfId="88" priority="33" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="92" priority="33" operator="lessThanOrEqual">
       <formula>H29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="87" priority="35" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="91" priority="35" operator="lessThanOrEqual">
       <formula>H30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="cellIs" dxfId="86" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="90" priority="1" operator="lessThanOrEqual">
       <formula>H7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="cellIs" dxfId="85" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="89" priority="3" operator="lessThanOrEqual">
       <formula>H8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="cellIs" dxfId="84" priority="5" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="88" priority="5" operator="lessThanOrEqual">
       <formula>H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="cellIs" dxfId="83" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="87" priority="8" operator="lessThanOrEqual">
       <formula>I10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="82" priority="10" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="86" priority="10" operator="lessThanOrEqual">
       <formula>I11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="cellIs" dxfId="81" priority="12" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="85" priority="12" operator="lessThanOrEqual">
       <formula>I13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="cellIs" dxfId="80" priority="14" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="84" priority="14" operator="lessThanOrEqual">
       <formula>I14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="cellIs" dxfId="79" priority="16" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="83" priority="16" operator="lessThanOrEqual">
       <formula>I15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="cellIs" dxfId="78" priority="18" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="82" priority="18" operator="lessThanOrEqual">
       <formula>I17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18">
-    <cfRule type="cellIs" dxfId="77" priority="20" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="81" priority="20" operator="lessThanOrEqual">
       <formula>I18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21">
-    <cfRule type="cellIs" dxfId="76" priority="22" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="80" priority="22" operator="lessThanOrEqual">
       <formula>I21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M22">
-    <cfRule type="cellIs" dxfId="75" priority="24" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="79" priority="24" operator="lessThanOrEqual">
       <formula>I22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24">
-    <cfRule type="cellIs" dxfId="74" priority="26" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="78" priority="26" operator="lessThanOrEqual">
       <formula>I24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M25">
-    <cfRule type="cellIs" dxfId="73" priority="28" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="77" priority="28" operator="lessThanOrEqual">
       <formula>I25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M27">
-    <cfRule type="cellIs" dxfId="72" priority="30" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="76" priority="30" operator="lessThanOrEqual">
       <formula>I27</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M28">
-    <cfRule type="cellIs" dxfId="71" priority="32" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="75" priority="32" operator="lessThanOrEqual">
       <formula>I28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M29">
-    <cfRule type="cellIs" dxfId="70" priority="34" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="74" priority="34" operator="lessThanOrEqual">
       <formula>I29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30">
-    <cfRule type="cellIs" dxfId="69" priority="36" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="73" priority="36" operator="lessThanOrEqual">
       <formula>I30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="68" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="72" priority="2" operator="lessThanOrEqual">
       <formula>I7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="67" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="71" priority="4" operator="lessThanOrEqual">
       <formula>I8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="cellIs" dxfId="66" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="70" priority="6" operator="lessThanOrEqual">
       <formula>I9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="65" priority="43" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="69" priority="43" operator="lessThanOrEqual">
       <formula>H10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11">
-    <cfRule type="cellIs" dxfId="64" priority="45" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="68" priority="45" operator="lessThanOrEqual">
       <formula>H11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R13">
-    <cfRule type="cellIs" dxfId="63" priority="47" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="67" priority="47" operator="lessThanOrEqual">
       <formula>H13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14">
-    <cfRule type="cellIs" dxfId="62" priority="49" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="66" priority="49" operator="lessThanOrEqual">
       <formula>H14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R15">
-    <cfRule type="cellIs" dxfId="61" priority="51" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="65" priority="51" operator="lessThanOrEqual">
       <formula>H15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17">
-    <cfRule type="cellIs" dxfId="60" priority="53" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="64" priority="53" operator="lessThanOrEqual">
       <formula>H17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R18">
-    <cfRule type="cellIs" dxfId="59" priority="55" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="63" priority="55" operator="lessThanOrEqual">
       <formula>H18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R19">
-    <cfRule type="cellIs" dxfId="58" priority="57" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="62" priority="57" operator="lessThanOrEqual">
       <formula>H19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R21">
-    <cfRule type="cellIs" dxfId="57" priority="59" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="61" priority="59" operator="lessThanOrEqual">
       <formula>H21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22">
-    <cfRule type="cellIs" dxfId="56" priority="61" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="60" priority="61" operator="lessThanOrEqual">
       <formula>H22</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="R23">
+    <cfRule type="cellIs" dxfId="59" priority="63" operator="lessThanOrEqual">
+      <formula>H23</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R24">
-    <cfRule type="cellIs" dxfId="55" priority="63" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="58" priority="65" operator="lessThanOrEqual">
       <formula>H24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R25">
-    <cfRule type="cellIs" dxfId="54" priority="65" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="57" priority="67" operator="lessThanOrEqual">
       <formula>H25</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="R26">
+    <cfRule type="cellIs" dxfId="56" priority="69" operator="lessThanOrEqual">
+      <formula>H26</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R28">
-    <cfRule type="cellIs" dxfId="53" priority="67" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="55" priority="71" operator="lessThanOrEqual">
       <formula>H28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R29">
-    <cfRule type="cellIs" dxfId="52" priority="69" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="54" priority="73" operator="lessThanOrEqual">
       <formula>H29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R30">
-    <cfRule type="cellIs" dxfId="51" priority="71" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="53" priority="75" operator="lessThanOrEqual">
       <formula>H30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="50" priority="37" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="52" priority="37" operator="lessThanOrEqual">
       <formula>H7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8">
-    <cfRule type="cellIs" dxfId="49" priority="39" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="51" priority="39" operator="lessThanOrEqual">
       <formula>H8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R9">
-    <cfRule type="cellIs" dxfId="48" priority="41" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="50" priority="41" operator="lessThanOrEqual">
       <formula>H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="47" priority="44" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="49" priority="44" operator="lessThanOrEqual">
       <formula>I10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S11">
-    <cfRule type="cellIs" dxfId="46" priority="46" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="48" priority="46" operator="lessThanOrEqual">
       <formula>I11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S13">
-    <cfRule type="cellIs" dxfId="45" priority="48" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="lessThanOrEqual">
       <formula>I13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14">
-    <cfRule type="cellIs" dxfId="44" priority="50" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="46" priority="50" operator="lessThanOrEqual">
       <formula>I14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S15">
-    <cfRule type="cellIs" dxfId="43" priority="52" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="45" priority="52" operator="lessThanOrEqual">
       <formula>I15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S17">
-    <cfRule type="cellIs" dxfId="42" priority="54" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="54" operator="lessThanOrEqual">
       <formula>I17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S18">
-    <cfRule type="cellIs" dxfId="41" priority="56" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="43" priority="56" operator="lessThanOrEqual">
       <formula>I18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S19">
-    <cfRule type="cellIs" dxfId="40" priority="58" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="42" priority="58" operator="lessThanOrEqual">
       <formula>I19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S21">
-    <cfRule type="cellIs" dxfId="39" priority="60" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="41" priority="60" operator="lessThanOrEqual">
       <formula>I21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22">
-    <cfRule type="cellIs" dxfId="38" priority="62" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="40" priority="62" operator="lessThanOrEqual">
       <formula>I22</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="S23">
+    <cfRule type="cellIs" dxfId="39" priority="64" operator="lessThanOrEqual">
+      <formula>I23</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="S24">
-    <cfRule type="cellIs" dxfId="37" priority="64" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="66" operator="lessThanOrEqual">
       <formula>I24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S25">
-    <cfRule type="cellIs" dxfId="36" priority="66" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="37" priority="68" operator="lessThanOrEqual">
       <formula>I25</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="S26">
+    <cfRule type="cellIs" dxfId="36" priority="70" operator="lessThanOrEqual">
+      <formula>I26</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="S28">
-    <cfRule type="cellIs" dxfId="35" priority="68" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="35" priority="72" operator="lessThanOrEqual">
       <formula>I28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S29">
-    <cfRule type="cellIs" dxfId="34" priority="70" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="74" operator="lessThanOrEqual">
       <formula>I29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S30">
-    <cfRule type="cellIs" dxfId="33" priority="72" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="33" priority="76" operator="lessThanOrEqual">
       <formula>I30</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4963,152 +5045,152 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X10">
-    <cfRule type="cellIs" dxfId="29" priority="79" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="29" priority="83" operator="lessThanOrEqual">
       <formula>H10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X11">
-    <cfRule type="cellIs" dxfId="28" priority="81" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="85" operator="lessThanOrEqual">
       <formula>H11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13">
-    <cfRule type="cellIs" dxfId="27" priority="83" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="27" priority="87" operator="lessThanOrEqual">
       <formula>H13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X14">
-    <cfRule type="cellIs" dxfId="26" priority="85" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="89" operator="lessThanOrEqual">
       <formula>H14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X15">
-    <cfRule type="cellIs" dxfId="25" priority="87" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="91" operator="lessThanOrEqual">
       <formula>H15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X18">
-    <cfRule type="cellIs" dxfId="24" priority="89" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="93" operator="lessThanOrEqual">
       <formula>H18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X21">
-    <cfRule type="cellIs" dxfId="23" priority="91" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="23" priority="95" operator="lessThanOrEqual">
       <formula>H21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X24">
-    <cfRule type="cellIs" dxfId="22" priority="93" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="97" operator="lessThanOrEqual">
       <formula>H24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X25">
-    <cfRule type="cellIs" dxfId="21" priority="95" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="21" priority="99" operator="lessThanOrEqual">
       <formula>H25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X28">
-    <cfRule type="cellIs" dxfId="20" priority="97" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="101" operator="lessThanOrEqual">
       <formula>H28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X29">
-    <cfRule type="cellIs" dxfId="19" priority="99" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="19" priority="103" operator="lessThanOrEqual">
       <formula>H29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X30">
-    <cfRule type="cellIs" dxfId="18" priority="101" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="105" operator="lessThanOrEqual">
       <formula>H30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X7">
-    <cfRule type="cellIs" dxfId="17" priority="73" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="77" operator="lessThanOrEqual">
       <formula>H7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X8">
-    <cfRule type="cellIs" dxfId="16" priority="75" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="79" operator="lessThanOrEqual">
       <formula>H8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X9">
-    <cfRule type="cellIs" dxfId="15" priority="77" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="81" operator="lessThanOrEqual">
       <formula>H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y10">
-    <cfRule type="cellIs" dxfId="14" priority="80" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="84" operator="lessThanOrEqual">
       <formula>I10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y11">
-    <cfRule type="cellIs" dxfId="13" priority="82" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="86" operator="lessThanOrEqual">
       <formula>I11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y13">
-    <cfRule type="cellIs" dxfId="12" priority="84" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="88" operator="lessThanOrEqual">
       <formula>I13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y14">
-    <cfRule type="cellIs" dxfId="11" priority="86" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="11" priority="90" operator="lessThanOrEqual">
       <formula>I14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y15">
-    <cfRule type="cellIs" dxfId="10" priority="88" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="92" operator="lessThanOrEqual">
       <formula>I15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y18">
-    <cfRule type="cellIs" dxfId="9" priority="90" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="94" operator="lessThanOrEqual">
       <formula>I18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y21">
-    <cfRule type="cellIs" dxfId="8" priority="92" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="96" operator="lessThanOrEqual">
       <formula>I21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y24">
-    <cfRule type="cellIs" dxfId="7" priority="94" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="98" operator="lessThanOrEqual">
       <formula>I24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y25">
-    <cfRule type="cellIs" dxfId="6" priority="96" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="100" operator="lessThanOrEqual">
       <formula>I25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y28">
-    <cfRule type="cellIs" dxfId="5" priority="98" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="102" operator="lessThanOrEqual">
       <formula>I28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y29">
-    <cfRule type="cellIs" dxfId="4" priority="100" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="104" operator="lessThanOrEqual">
       <formula>I29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y30">
-    <cfRule type="cellIs" dxfId="3" priority="102" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="106" operator="lessThanOrEqual">
       <formula>I30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y7">
-    <cfRule type="cellIs" dxfId="2" priority="74" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="78" operator="lessThanOrEqual">
       <formula>I7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y8">
-    <cfRule type="cellIs" dxfId="1" priority="76" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="80" operator="lessThanOrEqual">
       <formula>I8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9">
-    <cfRule type="cellIs" dxfId="0" priority="78" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="82" operator="lessThanOrEqual">
       <formula>I9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5148,24 +5230,26 @@
     <hyperlink ref="AA21" r:id="rId33"/>
     <hyperlink ref="O22" r:id="rId34"/>
     <hyperlink ref="U22" r:id="rId35"/>
-    <hyperlink ref="O24" r:id="rId36"/>
-    <hyperlink ref="U24" r:id="rId37"/>
-    <hyperlink ref="AA24" r:id="rId38"/>
-    <hyperlink ref="O25" r:id="rId39"/>
-    <hyperlink ref="U25" r:id="rId40"/>
-    <hyperlink ref="AA25" r:id="rId41"/>
-    <hyperlink ref="O27" r:id="rId42"/>
-    <hyperlink ref="O28" r:id="rId43"/>
-    <hyperlink ref="U28" r:id="rId44"/>
-    <hyperlink ref="AA28" r:id="rId45"/>
-    <hyperlink ref="O29" r:id="rId46"/>
-    <hyperlink ref="U29" r:id="rId47"/>
-    <hyperlink ref="AA29" r:id="rId48"/>
-    <hyperlink ref="O30" r:id="rId49"/>
-    <hyperlink ref="U30" r:id="rId50"/>
-    <hyperlink ref="AA30" r:id="rId51"/>
+    <hyperlink ref="U23" r:id="rId36"/>
+    <hyperlink ref="O24" r:id="rId37"/>
+    <hyperlink ref="U24" r:id="rId38"/>
+    <hyperlink ref="AA24" r:id="rId39"/>
+    <hyperlink ref="O25" r:id="rId40"/>
+    <hyperlink ref="U25" r:id="rId41"/>
+    <hyperlink ref="AA25" r:id="rId42"/>
+    <hyperlink ref="U26" r:id="rId43"/>
+    <hyperlink ref="O27" r:id="rId44"/>
+    <hyperlink ref="O28" r:id="rId45"/>
+    <hyperlink ref="U28" r:id="rId46"/>
+    <hyperlink ref="AA28" r:id="rId47"/>
+    <hyperlink ref="O29" r:id="rId48"/>
+    <hyperlink ref="U29" r:id="rId49"/>
+    <hyperlink ref="AA29" r:id="rId50"/>
+    <hyperlink ref="O30" r:id="rId51"/>
+    <hyperlink ref="U30" r:id="rId52"/>
+    <hyperlink ref="AA30" r:id="rId53"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId52"/>
+  <legacyDrawing r:id="rId54"/>
 </worksheet>
 </file>
</xml_diff>